<commit_message>
Add extra toxicity query
Add simple check for genes in toxicity-susceptible tissues - lists taken from the Human Protein Atlas.
</commit_message>
<xml_diff>
--- a/Data/Data manifest.xlsx
+++ b/Data/Data manifest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="152">
   <si>
     <t>Dataset</t>
   </si>
@@ -333,6 +333,150 @@
   </si>
   <si>
     <t xml:space="preserve">Reformatted version of https://www.uniprot.org/docs/pdbtosp.txt </t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/bone+marrow_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/bone+marrow_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/cervix_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/cervix_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/cervix_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/heart_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/heart_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/heart_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/kidney_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/kidney_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/kidney_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/liver_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/liver_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/liver_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/lymph+node_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/lymph+node_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/lymph+node_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/ovary_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/ovary_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/ovary_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/testis_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/testis_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/testis_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/bone+marrow_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Bone marrow at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Bone marrow at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Bone marrow at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Cervix at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Cervix at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Cervix at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Heart at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Heart at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Heart at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Kidney at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Kidney at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Kidney at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Liver at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Liver at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Liver at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Lymph node at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Lymph node at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Lymph node at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Ovary at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Ovary at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Ovary at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Testis at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Testis at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Testis at Tissue enriched level</t>
   </si>
 </sst>
 </file>
@@ -698,10 +842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,6 +1388,198 @@
       </c>
       <c r="E34" s="4">
         <v>43214</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>128</v>
+      </c>
+      <c r="B35" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>129</v>
+      </c>
+      <c r="B36" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>130</v>
+      </c>
+      <c r="B37" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>131</v>
+      </c>
+      <c r="B38" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>132</v>
+      </c>
+      <c r="B39" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>133</v>
+      </c>
+      <c r="B40" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>135</v>
+      </c>
+      <c r="B42" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>136</v>
+      </c>
+      <c r="B43" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>137</v>
+      </c>
+      <c r="B44" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>139</v>
+      </c>
+      <c r="B46" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>140</v>
+      </c>
+      <c r="B47" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>141</v>
+      </c>
+      <c r="B48" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>142</v>
+      </c>
+      <c r="B49" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>143</v>
+      </c>
+      <c r="B50" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>144</v>
+      </c>
+      <c r="B51" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>145</v>
+      </c>
+      <c r="B52" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>146</v>
+      </c>
+      <c r="B53" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>147</v>
+      </c>
+      <c r="B54" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>148</v>
+      </c>
+      <c r="B55" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>149</v>
+      </c>
+      <c r="B56" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>150</v>
+      </c>
+      <c r="B57" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>151</v>
+      </c>
+      <c r="B58" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add comparison to enriched gene lists from HPA
</commit_message>
<xml_diff>
--- a/Data/Data manifest.xlsx
+++ b/Data/Data manifest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="320">
   <si>
     <t>Dataset</t>
   </si>
@@ -477,6 +477,510 @@
   </si>
   <si>
     <t>Human Protein Atlas: RNA expression in Testis at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:bone+marrow;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:bone+marrow;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:bone+marrow;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:cervix;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:cervix;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:cervix;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:heart;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:heart;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:heart;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:kidney;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:kidney;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:kidney;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:liver;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:liver;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:liver;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:lymph+node;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:lymph+node;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:lymph+node;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:ovary;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:ovary;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:ovary;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:testis;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:testis;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:testis;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/adipose_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/adipose_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/adrenal+gland_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/adrenal+gland_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/adrenal+gland_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/appendix_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/appendix_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/appendix_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/brain_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/brain_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/brain_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/breast_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/breast_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/breast_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/colon_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/colon_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/colon_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/duodenum_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/duodenum_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/duodenum_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/endometrium_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/endometrium_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/endometrium_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/epididymis_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/epididymis_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/epididymis_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/esophagus_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/esophagus_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/esophagus_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/gallbladder_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/gallbladder_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/gallbladder_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/lung_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/lung_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/lung_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/pancreas_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/pancreas_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/pancreas_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/parathyroid+gland_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/parathyroid+gland_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/parathyroid+gland_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/placenta_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/placenta_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/placenta_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/prostate_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/prostate_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/prostate_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/salivary+gland_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/salivary+gland_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/salivary+gland_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/seminal+vesicle_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/seminal+vesicle_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/seminal+vesicle_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/skeletal+muscle_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/skeletal+muscle_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/skeletal+muscle_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/skin_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/skin_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/skin_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/small+intestine_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/small+intestine_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/small+intestine_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/spleen_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/spleen_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/spleen_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/stomach_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/stomach_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/stomach_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/thyroid+gland_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/thyroid+gland_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/thyroid+gland_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/adipose_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:adipose;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:adipose;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:adipose;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:adrenal+gland;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:adrenal+gland;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:adrenal+gland;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:appendix;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:appendix;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:appendix;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:brain;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:brain;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:brain;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:breast;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:breast;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:breast;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:colon;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:colon;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:colon;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:duodenum;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:duodenum;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:duodenum;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:endometrium;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:endometrium;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:endometrium;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:epididymis;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:epididymis;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:epididymis;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:esophagus;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:esophagus;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:esophagus;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:gallbladder;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:gallbladder;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:gallbladder;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:lung;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:lung;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:lung;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:pancreas;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:pancreas;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:pancreas;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:parathyroid+gland;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:parathyroid+gland;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:parathyroid+gland;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:placenta;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:placenta;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:placenta;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:prostate;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:prostate;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:prostate;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:salivary+gland;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:salivary+gland;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:salivary+gland;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:seminal+vesicle;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:seminal+vesicle;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:seminal+vesicle;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:skeletal+muscle;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:skeletal+muscle;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:skeletal+muscle;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:skin;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:skin;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:skin;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:small+intestine;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:small+intestine;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:small+intestine;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:spleen;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:spleen;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:spleen;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:stomach;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:stomach;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:stomach;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:thyroid+gland;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:thyroid+gland;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:thyroid+gland;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
   </si>
 </sst>
 </file>
@@ -842,10 +1346,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="B97" workbookViewId="0">
+      <selection activeCell="H123" sqref="H123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,7 +1899,13 @@
         <v>128</v>
       </c>
       <c r="B35" t="s">
-        <v>127</v>
+        <v>247</v>
+      </c>
+      <c r="C35" t="s">
+        <v>248</v>
+      </c>
+      <c r="E35" s="4">
+        <v>43244</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1403,7 +1913,13 @@
         <v>129</v>
       </c>
       <c r="B36" t="s">
-        <v>104</v>
+        <v>176</v>
+      </c>
+      <c r="C36" t="s">
+        <v>249</v>
+      </c>
+      <c r="E36" s="4">
+        <v>43244</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1411,7 +1927,13 @@
         <v>130</v>
       </c>
       <c r="B37" t="s">
-        <v>105</v>
+        <v>177</v>
+      </c>
+      <c r="C37" t="s">
+        <v>250</v>
+      </c>
+      <c r="E37" s="4">
+        <v>43244</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1419,7 +1941,13 @@
         <v>131</v>
       </c>
       <c r="B38" t="s">
-        <v>106</v>
+        <v>178</v>
+      </c>
+      <c r="C38" t="s">
+        <v>251</v>
+      </c>
+      <c r="E38" s="4">
+        <v>43244</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1427,7 +1955,13 @@
         <v>132</v>
       </c>
       <c r="B39" t="s">
-        <v>107</v>
+        <v>179</v>
+      </c>
+      <c r="C39" t="s">
+        <v>252</v>
+      </c>
+      <c r="E39" s="4">
+        <v>43244</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1435,7 +1969,13 @@
         <v>133</v>
       </c>
       <c r="B40" t="s">
-        <v>108</v>
+        <v>180</v>
+      </c>
+      <c r="C40" t="s">
+        <v>253</v>
+      </c>
+      <c r="E40" s="4">
+        <v>43244</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1443,7 +1983,13 @@
         <v>134</v>
       </c>
       <c r="B41" t="s">
-        <v>109</v>
+        <v>181</v>
+      </c>
+      <c r="C41" t="s">
+        <v>254</v>
+      </c>
+      <c r="E41" s="4">
+        <v>43244</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1451,7 +1997,13 @@
         <v>135</v>
       </c>
       <c r="B42" t="s">
-        <v>110</v>
+        <v>182</v>
+      </c>
+      <c r="C42" t="s">
+        <v>255</v>
+      </c>
+      <c r="E42" s="4">
+        <v>43244</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1459,7 +2011,13 @@
         <v>136</v>
       </c>
       <c r="B43" t="s">
-        <v>111</v>
+        <v>183</v>
+      </c>
+      <c r="C43" t="s">
+        <v>256</v>
+      </c>
+      <c r="E43" s="4">
+        <v>43244</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1467,7 +2025,13 @@
         <v>137</v>
       </c>
       <c r="B44" t="s">
-        <v>112</v>
+        <v>127</v>
+      </c>
+      <c r="C44" t="s">
+        <v>152</v>
+      </c>
+      <c r="E44" s="4">
+        <v>43244</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1475,7 +2039,13 @@
         <v>138</v>
       </c>
       <c r="B45" t="s">
-        <v>113</v>
+        <v>104</v>
+      </c>
+      <c r="C45" t="s">
+        <v>153</v>
+      </c>
+      <c r="E45" s="4">
+        <v>43244</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1483,7 +2053,13 @@
         <v>139</v>
       </c>
       <c r="B46" t="s">
-        <v>114</v>
+        <v>105</v>
+      </c>
+      <c r="C46" t="s">
+        <v>154</v>
+      </c>
+      <c r="E46" s="4">
+        <v>43244</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1491,7 +2067,13 @@
         <v>140</v>
       </c>
       <c r="B47" t="s">
-        <v>115</v>
+        <v>184</v>
+      </c>
+      <c r="C47" t="s">
+        <v>257</v>
+      </c>
+      <c r="E47" s="4">
+        <v>43244</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1499,87 +2081,945 @@
         <v>141</v>
       </c>
       <c r="B48" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+      <c r="C48" t="s">
+        <v>258</v>
+      </c>
+      <c r="E48" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>142</v>
       </c>
       <c r="B49" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="C49" t="s">
+        <v>259</v>
+      </c>
+      <c r="E49" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>143</v>
       </c>
       <c r="B50" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+      <c r="C50" t="s">
+        <v>260</v>
+      </c>
+      <c r="E50" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>144</v>
       </c>
       <c r="B51" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="C51" t="s">
+        <v>261</v>
+      </c>
+      <c r="E51" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>145</v>
       </c>
       <c r="B52" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+      <c r="C52" t="s">
+        <v>262</v>
+      </c>
+      <c r="E52" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>146</v>
       </c>
       <c r="B53" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="C53" t="s">
+        <v>155</v>
+      </c>
+      <c r="E53" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>147</v>
       </c>
       <c r="B54" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="C54" t="s">
+        <v>156</v>
+      </c>
+      <c r="E54" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>148</v>
       </c>
       <c r="B55" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="C55" t="s">
+        <v>157</v>
+      </c>
+      <c r="E55" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>149</v>
       </c>
       <c r="B56" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+      <c r="C56" t="s">
+        <v>263</v>
+      </c>
+      <c r="E56" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>150</v>
       </c>
       <c r="B57" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+      <c r="C57" t="s">
+        <v>264</v>
+      </c>
+      <c r="E57" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>151</v>
       </c>
       <c r="B58" t="s">
+        <v>192</v>
+      </c>
+      <c r="C58" t="s">
+        <v>265</v>
+      </c>
+      <c r="E58" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>193</v>
+      </c>
+      <c r="C59" t="s">
+        <v>266</v>
+      </c>
+      <c r="E59" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>194</v>
+      </c>
+      <c r="C60" t="s">
+        <v>267</v>
+      </c>
+      <c r="E60" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>195</v>
+      </c>
+      <c r="C61" t="s">
+        <v>268</v>
+      </c>
+      <c r="E61" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>196</v>
+      </c>
+      <c r="C62" t="s">
+        <v>269</v>
+      </c>
+      <c r="E62" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>197</v>
+      </c>
+      <c r="C63" t="s">
+        <v>270</v>
+      </c>
+      <c r="E63" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>198</v>
+      </c>
+      <c r="C64" t="s">
+        <v>271</v>
+      </c>
+      <c r="E64" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>199</v>
+      </c>
+      <c r="C65" t="s">
+        <v>272</v>
+      </c>
+      <c r="E65" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>200</v>
+      </c>
+      <c r="C66" t="s">
+        <v>273</v>
+      </c>
+      <c r="E66" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>201</v>
+      </c>
+      <c r="C67" t="s">
+        <v>274</v>
+      </c>
+      <c r="E67" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>202</v>
+      </c>
+      <c r="C68" t="s">
+        <v>275</v>
+      </c>
+      <c r="E68" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>203</v>
+      </c>
+      <c r="C69" t="s">
+        <v>276</v>
+      </c>
+      <c r="E69" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>204</v>
+      </c>
+      <c r="C70" t="s">
+        <v>277</v>
+      </c>
+      <c r="E70" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>205</v>
+      </c>
+      <c r="C71" t="s">
+        <v>278</v>
+      </c>
+      <c r="E71" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>206</v>
+      </c>
+      <c r="C72" t="s">
+        <v>279</v>
+      </c>
+      <c r="E72" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>207</v>
+      </c>
+      <c r="C73" t="s">
+        <v>280</v>
+      </c>
+      <c r="E73" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>109</v>
+      </c>
+      <c r="C74" t="s">
+        <v>158</v>
+      </c>
+      <c r="E74" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>110</v>
+      </c>
+      <c r="C75" t="s">
+        <v>159</v>
+      </c>
+      <c r="E75" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>111</v>
+      </c>
+      <c r="C76" t="s">
+        <v>160</v>
+      </c>
+      <c r="E76" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>112</v>
+      </c>
+      <c r="C77" t="s">
+        <v>161</v>
+      </c>
+      <c r="E77" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>113</v>
+      </c>
+      <c r="C78" t="s">
+        <v>162</v>
+      </c>
+      <c r="E78" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>114</v>
+      </c>
+      <c r="C79" t="s">
+        <v>163</v>
+      </c>
+      <c r="E79" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>115</v>
+      </c>
+      <c r="C80" t="s">
+        <v>164</v>
+      </c>
+      <c r="E80" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>116</v>
+      </c>
+      <c r="C81" t="s">
+        <v>165</v>
+      </c>
+      <c r="E81" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>117</v>
+      </c>
+      <c r="C82" t="s">
+        <v>166</v>
+      </c>
+      <c r="E82" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>208</v>
+      </c>
+      <c r="C83" t="s">
+        <v>281</v>
+      </c>
+      <c r="E83" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>209</v>
+      </c>
+      <c r="C84" t="s">
+        <v>282</v>
+      </c>
+      <c r="E84" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>210</v>
+      </c>
+      <c r="C85" t="s">
+        <v>283</v>
+      </c>
+      <c r="E85" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>118</v>
+      </c>
+      <c r="C86" t="s">
+        <v>167</v>
+      </c>
+      <c r="E86" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>119</v>
+      </c>
+      <c r="C87" t="s">
+        <v>168</v>
+      </c>
+      <c r="E87" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>120</v>
+      </c>
+      <c r="C88" t="s">
+        <v>169</v>
+      </c>
+      <c r="E88" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>121</v>
+      </c>
+      <c r="C89" t="s">
+        <v>170</v>
+      </c>
+      <c r="E89" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>122</v>
+      </c>
+      <c r="C90" t="s">
+        <v>171</v>
+      </c>
+      <c r="E90" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>123</v>
+      </c>
+      <c r="C91" t="s">
+        <v>172</v>
+      </c>
+      <c r="E91" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>211</v>
+      </c>
+      <c r="C92" t="s">
+        <v>284</v>
+      </c>
+      <c r="E92" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>212</v>
+      </c>
+      <c r="C93" t="s">
+        <v>285</v>
+      </c>
+      <c r="E93" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>213</v>
+      </c>
+      <c r="C94" t="s">
+        <v>286</v>
+      </c>
+      <c r="E94" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>214</v>
+      </c>
+      <c r="C95" t="s">
+        <v>287</v>
+      </c>
+      <c r="E95" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>215</v>
+      </c>
+      <c r="C96" t="s">
+        <v>288</v>
+      </c>
+      <c r="E96" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>216</v>
+      </c>
+      <c r="C97" t="s">
+        <v>289</v>
+      </c>
+      <c r="E97" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>217</v>
+      </c>
+      <c r="C98" t="s">
+        <v>290</v>
+      </c>
+      <c r="E98" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>218</v>
+      </c>
+      <c r="C99" t="s">
+        <v>291</v>
+      </c>
+      <c r="E99" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>219</v>
+      </c>
+      <c r="C100" t="s">
+        <v>292</v>
+      </c>
+      <c r="E100" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>220</v>
+      </c>
+      <c r="C101" t="s">
+        <v>293</v>
+      </c>
+      <c r="E101" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>221</v>
+      </c>
+      <c r="C102" t="s">
+        <v>294</v>
+      </c>
+      <c r="E102" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>222</v>
+      </c>
+      <c r="C103" t="s">
+        <v>295</v>
+      </c>
+      <c r="E103" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>223</v>
+      </c>
+      <c r="C104" t="s">
+        <v>296</v>
+      </c>
+      <c r="E104" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>224</v>
+      </c>
+      <c r="C105" t="s">
+        <v>297</v>
+      </c>
+      <c r="E105" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>225</v>
+      </c>
+      <c r="C106" t="s">
+        <v>298</v>
+      </c>
+      <c r="E106" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>226</v>
+      </c>
+      <c r="C107" t="s">
+        <v>299</v>
+      </c>
+      <c r="E107" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>227</v>
+      </c>
+      <c r="C108" t="s">
+        <v>300</v>
+      </c>
+      <c r="E108" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>228</v>
+      </c>
+      <c r="C109" t="s">
+        <v>301</v>
+      </c>
+      <c r="E109" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>229</v>
+      </c>
+      <c r="C110" t="s">
+        <v>302</v>
+      </c>
+      <c r="E110" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>230</v>
+      </c>
+      <c r="C111" t="s">
+        <v>303</v>
+      </c>
+      <c r="E111" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="112" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>231</v>
+      </c>
+      <c r="C112" t="s">
+        <v>304</v>
+      </c>
+      <c r="E112" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>232</v>
+      </c>
+      <c r="C113" t="s">
+        <v>305</v>
+      </c>
+      <c r="E113" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>233</v>
+      </c>
+      <c r="C114" t="s">
+        <v>306</v>
+      </c>
+      <c r="E114" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>234</v>
+      </c>
+      <c r="C115" t="s">
+        <v>307</v>
+      </c>
+      <c r="E115" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>235</v>
+      </c>
+      <c r="C116" t="s">
+        <v>308</v>
+      </c>
+      <c r="E116" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>236</v>
+      </c>
+      <c r="C117" t="s">
+        <v>309</v>
+      </c>
+      <c r="E117" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>237</v>
+      </c>
+      <c r="C118" t="s">
+        <v>310</v>
+      </c>
+      <c r="E118" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B119" t="s">
+        <v>238</v>
+      </c>
+      <c r="C119" t="s">
+        <v>311</v>
+      </c>
+      <c r="E119" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
+        <v>239</v>
+      </c>
+      <c r="C120" t="s">
+        <v>312</v>
+      </c>
+      <c r="E120" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
+        <v>240</v>
+      </c>
+      <c r="C121" t="s">
+        <v>313</v>
+      </c>
+      <c r="E121" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
+        <v>241</v>
+      </c>
+      <c r="C122" t="s">
+        <v>314</v>
+      </c>
+      <c r="E122" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B123" t="s">
+        <v>242</v>
+      </c>
+      <c r="C123" t="s">
+        <v>315</v>
+      </c>
+      <c r="E123" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
+        <v>243</v>
+      </c>
+      <c r="C124" t="s">
+        <v>316</v>
+      </c>
+      <c r="E124" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
+        <v>124</v>
+      </c>
+      <c r="C125" t="s">
+        <v>173</v>
+      </c>
+      <c r="E125" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B126" t="s">
+        <v>125</v>
+      </c>
+      <c r="C126" t="s">
+        <v>174</v>
+      </c>
+      <c r="E126" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B127" t="s">
         <v>126</v>
+      </c>
+      <c r="C127" t="s">
+        <v>175</v>
+      </c>
+      <c r="E127" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="128" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
+        <v>244</v>
+      </c>
+      <c r="C128" t="s">
+        <v>317</v>
+      </c>
+      <c r="E128" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
+        <v>245</v>
+      </c>
+      <c r="C129" t="s">
+        <v>318</v>
+      </c>
+      <c r="E129" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
+        <v>246</v>
+      </c>
+      <c r="C130" t="s">
+        <v>319</v>
+      </c>
+      <c r="E130" s="4">
+        <v>43244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Add data from IUPHAR concerning ligand interactions. -Bug fixes to SM druggability and AB-ability bucketing, to better make use of available information.
</commit_message>
<xml_diff>
--- a/Data/Data manifest.xlsx
+++ b/Data/Data manifest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="323">
   <si>
     <t>Dataset</t>
   </si>
@@ -981,6 +981,15 @@
   </si>
   <si>
     <t>https://www.proteinatlas.org/search/tissue_specificity_rna:thyroid+gland;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>Data/IUPHAR_ligand-gene_interactions.csv</t>
+  </si>
+  <si>
+    <t>http://www.guidetopharmacology.org/download.jsp</t>
+  </si>
+  <si>
+    <t>https://dx.doi.org/10.1093%2Fnar%2Fgks960</t>
   </si>
 </sst>
 </file>
@@ -1346,10 +1355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E130"/>
+  <dimension ref="A1:E131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B97" workbookViewId="0">
-      <selection activeCell="H123" sqref="H123"/>
+    <sheetView tabSelected="1" topLeftCell="B115" workbookViewId="0">
+      <selection activeCell="D134" sqref="D134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3020,6 +3029,20 @@
       </c>
       <c r="E130" s="4">
         <v>43244</v>
+      </c>
+    </row>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
+        <v>320</v>
+      </c>
+      <c r="C131" t="s">
+        <v>321</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E131" s="4">
+        <v>43333</v>
       </c>
     </row>
   </sheetData>
@@ -3039,9 +3062,10 @@
     <hyperlink ref="D25" r:id="rId13" display="https://doi.org/10.1093/nar/gkw1039"/>
     <hyperlink ref="D33" r:id="rId14"/>
     <hyperlink ref="D34" r:id="rId15"/>
+    <hyperlink ref="D131" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add VerSeDa secretome data
</commit_message>
<xml_diff>
--- a/Data/Data manifest.xlsx
+++ b/Data/Data manifest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="326">
   <si>
     <t>Dataset</t>
   </si>
@@ -990,6 +990,15 @@
   </si>
   <si>
     <t>https://dx.doi.org/10.1093%2Fnar%2Fgks960</t>
+  </si>
+  <si>
+    <t>Data/VerSeDa_HSapiens_secretedProteins.csv</t>
+  </si>
+  <si>
+    <t>http://genomics.cicbiogune.es/VerSeDa/index.php - SecretomeP = 0.9</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5467544/</t>
   </si>
 </sst>
 </file>
@@ -1355,10 +1364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E131"/>
+  <dimension ref="A1:E132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B115" workbookViewId="0">
-      <selection activeCell="D134" sqref="D134"/>
+    <sheetView tabSelected="1" topLeftCell="B112" workbookViewId="0">
+      <selection activeCell="E132" sqref="E132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3043,6 +3052,20 @@
       </c>
       <c r="E131" s="4">
         <v>43333</v>
+      </c>
+    </row>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
+        <v>323</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D132" t="s">
+        <v>325</v>
+      </c>
+      <c r="E132" s="4">
+        <v>43335</v>
       </c>
     </row>
   </sheetData>
@@ -3063,9 +3086,10 @@
     <hyperlink ref="D33" r:id="rId14"/>
     <hyperlink ref="D34" r:id="rId15"/>
     <hyperlink ref="D131" r:id="rId16"/>
+    <hyperlink ref="C132" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Replace queries to deactivated DrugEBIlity service Add data from wikipathways Add GnomAD query Update deprecated Pandas functions
</commit_message>
<xml_diff>
--- a/Data/Data manifest.xlsx
+++ b/Data/Data manifest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="444">
   <si>
     <t>Dataset</t>
   </si>
@@ -1023,6 +1023,336 @@
   </si>
   <si>
     <t>data_utils/make_chembl_targets_data.py</t>
+  </si>
+  <si>
+    <t>Data/domain_details.txt</t>
+  </si>
+  <si>
+    <t>Data/domain_drugebility.txt</t>
+  </si>
+  <si>
+    <t>ftp://ftp.ebi.ac.uk/pub/databases/chembl/DrugEBIlity/releases/3.0/</t>
+  </si>
+  <si>
+    <t>Data/gnomad.v2.1.1.lof_metrics.by_gene.txt</t>
+  </si>
+  <si>
+    <t>https://gnomad.broadinstitute.org/</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/adipose+tissue_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/adipose+tissue_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/adipose+tissue_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Adipose tissue at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Adipose tissue at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Adipose tissue at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Adrenal gland at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression inAdrenal gland at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Adrenal gland at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Cerebral cortex at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Cerebral cortex at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Cerebral cortex at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/cerebral+cortex_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/cerebral+cortex_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/cerebral+cortex_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:cerebral_cortex;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:cerebral_cortex;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:cerebral_cortex;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Cervix, uterine at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Cervix, uterine at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Cervix, uterine at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/cervix,+uterine_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/cervix,+uterine_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/cervix,+uterine_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:cervix,+uterine;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:cervix,+uterine;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:cervix,+uterine;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Heart muscle at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Heart muscle at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Heart muscle at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/heart+muscle_Group+enriched.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/heart+muscle_Tissue+enhanced.csv</t>
+  </si>
+  <si>
+    <t>Data/HPA_tox_lists/heart+muscle_Tissue+enriched.csv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:heart+muscle;Group+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:heart+muscle;Tissue+enhanced+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/search/tissue_specificity_rna:heart+muscle;Tissue+enriched+AND+sort_by:tissue+specific+score?format=tsv</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Appendix at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Brain at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Brain at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Brain at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Breast at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Breast at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Breast at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Colon at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Colon at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Appendix at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Appendix at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Colon at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Duodenum at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Duodenum at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Duodenum at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Endometrium at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Endometrium at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Endometrium at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Epididymis at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Epididymis at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Epididymis at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Esophagus at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Esophagus at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Esophagus at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Gall bladder at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Gall bladder at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Gall bladder at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Lung at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Lung at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Lung at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Pancreas at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Pancreas at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Pancreas at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Parathyroid at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Parathyroid at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Parathyroid at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Placenta at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Placenta at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Placenta at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Prostate at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Prostate at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Prostate at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Salivary gland at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Salivary gland at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Salivary gland at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Seminal vesicle at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Seminal vesicle at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Seminal vesicle at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Skeletal muscle at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Skeletal muscle at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Skeletal muscle at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Skin at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Skin at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Skin at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Small intestine at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Small intestine at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Small intestine at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Spleen at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Spleen at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Spleen at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Stomach at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Stomach at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Stomach at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Thyroid gland at Group enriched level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Thyroid gland at Tissue enhanced level</t>
+  </si>
+  <si>
+    <t>Human Protein Atlas: RNA expression in Thyroid gland at Tissue enriched level</t>
+  </si>
+  <si>
+    <t>Human genes producing proteins identified in VerSeDa as being secreted</t>
+  </si>
+  <si>
+    <t>A lookup table of various  identifiers for genes</t>
+  </si>
+  <si>
+    <t>A data dump from EBI's now discontinued DrugEBIlity tool</t>
   </si>
 </sst>
 </file>
@@ -1388,10 +1718,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F133"/>
+  <dimension ref="A1:F148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B103" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1960,7 +2291,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>128</v>
+        <v>342</v>
       </c>
       <c r="B35" t="s">
         <v>247</v>
@@ -1974,7 +2305,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>129</v>
+        <v>343</v>
       </c>
       <c r="B36" t="s">
         <v>176</v>
@@ -1988,7 +2319,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>130</v>
+        <v>344</v>
       </c>
       <c r="B37" t="s">
         <v>177</v>
@@ -2002,13 +2333,13 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>131</v>
+        <v>342</v>
       </c>
       <c r="B38" t="s">
-        <v>178</v>
+        <v>339</v>
       </c>
       <c r="D38" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F38" s="4">
         <v>43244</v>
@@ -2016,13 +2347,13 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>132</v>
+        <v>343</v>
       </c>
       <c r="B39" t="s">
-        <v>179</v>
+        <v>340</v>
       </c>
       <c r="D39" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F39" s="4">
         <v>43244</v>
@@ -2030,13 +2361,13 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>133</v>
+        <v>344</v>
       </c>
       <c r="B40" t="s">
-        <v>180</v>
+        <v>341</v>
       </c>
       <c r="D40" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F40" s="4">
         <v>43244</v>
@@ -2044,13 +2375,13 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>134</v>
+        <v>345</v>
       </c>
       <c r="B41" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D41" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F41" s="4">
         <v>43244</v>
@@ -2058,13 +2389,13 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>135</v>
+        <v>346</v>
       </c>
       <c r="B42" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D42" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F42" s="4">
         <v>43244</v>
@@ -2072,13 +2403,13 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>136</v>
+        <v>347</v>
       </c>
       <c r="B43" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D43" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F43" s="4">
         <v>43244</v>
@@ -2086,13 +2417,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>137</v>
+        <v>375</v>
       </c>
       <c r="B44" t="s">
-        <v>127</v>
+        <v>181</v>
       </c>
       <c r="D44" t="s">
-        <v>152</v>
+        <v>254</v>
       </c>
       <c r="F44" s="4">
         <v>43244</v>
@@ -2100,13 +2431,13 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>138</v>
+        <v>384</v>
       </c>
       <c r="B45" t="s">
-        <v>104</v>
+        <v>182</v>
       </c>
       <c r="D45" t="s">
-        <v>153</v>
+        <v>255</v>
       </c>
       <c r="F45" s="4">
         <v>43244</v>
@@ -2114,13 +2445,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>139</v>
+        <v>385</v>
       </c>
       <c r="B46" t="s">
-        <v>105</v>
+        <v>183</v>
       </c>
       <c r="D46" t="s">
-        <v>154</v>
+        <v>256</v>
       </c>
       <c r="F46" s="4">
         <v>43244</v>
@@ -2128,13 +2459,13 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="B47" t="s">
-        <v>184</v>
+        <v>127</v>
       </c>
       <c r="D47" t="s">
-        <v>257</v>
+        <v>152</v>
       </c>
       <c r="F47" s="4">
         <v>43244</v>
@@ -2142,13 +2473,13 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="B48" t="s">
-        <v>185</v>
+        <v>104</v>
       </c>
       <c r="D48" t="s">
-        <v>258</v>
+        <v>153</v>
       </c>
       <c r="F48" s="4">
         <v>43244</v>
@@ -2156,13 +2487,13 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B49" t="s">
-        <v>186</v>
+        <v>105</v>
       </c>
       <c r="D49" t="s">
-        <v>259</v>
+        <v>154</v>
       </c>
       <c r="F49" s="4">
         <v>43244</v>
@@ -2170,13 +2501,13 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>143</v>
+        <v>376</v>
       </c>
       <c r="B50" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D50" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F50" s="4">
         <v>43244</v>
@@ -2184,13 +2515,13 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>144</v>
+        <v>377</v>
       </c>
       <c r="B51" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D51" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F51" s="4">
         <v>43244</v>
@@ -2198,13 +2529,13 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>145</v>
+        <v>378</v>
       </c>
       <c r="B52" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D52" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F52" s="4">
         <v>43244</v>
@@ -2212,13 +2543,13 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>146</v>
+        <v>379</v>
       </c>
       <c r="B53" t="s">
-        <v>106</v>
+        <v>187</v>
       </c>
       <c r="D53" t="s">
-        <v>155</v>
+        <v>260</v>
       </c>
       <c r="F53" s="4">
         <v>43244</v>
@@ -2226,13 +2557,13 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>147</v>
+        <v>380</v>
       </c>
       <c r="B54" t="s">
-        <v>107</v>
+        <v>188</v>
       </c>
       <c r="D54" t="s">
-        <v>156</v>
+        <v>261</v>
       </c>
       <c r="F54" s="4">
         <v>43244</v>
@@ -2240,13 +2571,13 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>148</v>
+        <v>381</v>
       </c>
       <c r="B55" t="s">
-        <v>108</v>
+        <v>189</v>
       </c>
       <c r="D55" t="s">
-        <v>157</v>
+        <v>262</v>
       </c>
       <c r="F55" s="4">
         <v>43244</v>
@@ -2254,13 +2585,13 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>149</v>
+        <v>348</v>
       </c>
       <c r="B56" t="s">
-        <v>190</v>
+        <v>351</v>
       </c>
       <c r="D56" t="s">
-        <v>263</v>
+        <v>354</v>
       </c>
       <c r="F56" s="4">
         <v>43244</v>
@@ -2268,13 +2599,13 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>150</v>
+        <v>349</v>
       </c>
       <c r="B57" t="s">
-        <v>191</v>
+        <v>352</v>
       </c>
       <c r="D57" t="s">
-        <v>264</v>
+        <v>355</v>
       </c>
       <c r="F57" s="4">
         <v>43244</v>
@@ -2282,847 +2613,1273 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>350</v>
+      </c>
+      <c r="B58" t="s">
+        <v>353</v>
+      </c>
+      <c r="D58" t="s">
+        <v>356</v>
+      </c>
+      <c r="F58" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>131</v>
+      </c>
+      <c r="B59" t="s">
+        <v>106</v>
+      </c>
+      <c r="D59" t="s">
+        <v>155</v>
+      </c>
+      <c r="F59" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>132</v>
+      </c>
+      <c r="B60" t="s">
+        <v>107</v>
+      </c>
+      <c r="D60" t="s">
+        <v>156</v>
+      </c>
+      <c r="F60" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>133</v>
+      </c>
+      <c r="B61" t="s">
+        <v>108</v>
+      </c>
+      <c r="D61" t="s">
+        <v>157</v>
+      </c>
+      <c r="F61" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>357</v>
+      </c>
+      <c r="B62" t="s">
+        <v>360</v>
+      </c>
+      <c r="D62" t="s">
+        <v>363</v>
+      </c>
+      <c r="F62" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>358</v>
+      </c>
+      <c r="B63" t="s">
+        <v>361</v>
+      </c>
+      <c r="D63" t="s">
+        <v>364</v>
+      </c>
+      <c r="F63" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>359</v>
+      </c>
+      <c r="B64" t="s">
+        <v>362</v>
+      </c>
+      <c r="D64" t="s">
+        <v>365</v>
+      </c>
+      <c r="F64" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>382</v>
+      </c>
+      <c r="B65" t="s">
+        <v>190</v>
+      </c>
+      <c r="D65" t="s">
+        <v>263</v>
+      </c>
+      <c r="F65" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>383</v>
+      </c>
+      <c r="B66" t="s">
+        <v>191</v>
+      </c>
+      <c r="D66" t="s">
+        <v>264</v>
+      </c>
+      <c r="F66" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>386</v>
+      </c>
+      <c r="B67" t="s">
+        <v>192</v>
+      </c>
+      <c r="D67" t="s">
+        <v>265</v>
+      </c>
+      <c r="F67" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>387</v>
+      </c>
+      <c r="B68" t="s">
+        <v>193</v>
+      </c>
+      <c r="D68" t="s">
+        <v>266</v>
+      </c>
+      <c r="F68" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>388</v>
+      </c>
+      <c r="B69" t="s">
+        <v>194</v>
+      </c>
+      <c r="D69" t="s">
+        <v>267</v>
+      </c>
+      <c r="F69" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>389</v>
+      </c>
+      <c r="B70" t="s">
+        <v>195</v>
+      </c>
+      <c r="D70" t="s">
+        <v>268</v>
+      </c>
+      <c r="F70" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>390</v>
+      </c>
+      <c r="B71" t="s">
+        <v>196</v>
+      </c>
+      <c r="D71" t="s">
+        <v>269</v>
+      </c>
+      <c r="F71" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>391</v>
+      </c>
+      <c r="B72" t="s">
+        <v>197</v>
+      </c>
+      <c r="D72" t="s">
+        <v>270</v>
+      </c>
+      <c r="F72" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>392</v>
+      </c>
+      <c r="B73" t="s">
+        <v>198</v>
+      </c>
+      <c r="D73" t="s">
+        <v>271</v>
+      </c>
+      <c r="F73" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>393</v>
+      </c>
+      <c r="B74" t="s">
+        <v>199</v>
+      </c>
+      <c r="D74" t="s">
+        <v>272</v>
+      </c>
+      <c r="F74" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>394</v>
+      </c>
+      <c r="B75" t="s">
+        <v>200</v>
+      </c>
+      <c r="D75" t="s">
+        <v>273</v>
+      </c>
+      <c r="F75" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>395</v>
+      </c>
+      <c r="B76" t="s">
+        <v>201</v>
+      </c>
+      <c r="D76" t="s">
+        <v>274</v>
+      </c>
+      <c r="F76" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>396</v>
+      </c>
+      <c r="B77" t="s">
+        <v>202</v>
+      </c>
+      <c r="D77" t="s">
+        <v>275</v>
+      </c>
+      <c r="F77" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>397</v>
+      </c>
+      <c r="B78" t="s">
+        <v>203</v>
+      </c>
+      <c r="D78" t="s">
+        <v>276</v>
+      </c>
+      <c r="F78" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>398</v>
+      </c>
+      <c r="B79" t="s">
+        <v>204</v>
+      </c>
+      <c r="D79" t="s">
+        <v>277</v>
+      </c>
+      <c r="F79" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>399</v>
+      </c>
+      <c r="B80" t="s">
+        <v>205</v>
+      </c>
+      <c r="D80" t="s">
+        <v>278</v>
+      </c>
+      <c r="F80" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>400</v>
+      </c>
+      <c r="B81" t="s">
+        <v>206</v>
+      </c>
+      <c r="D81" t="s">
+        <v>279</v>
+      </c>
+      <c r="F81" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>401</v>
+      </c>
+      <c r="B82" t="s">
+        <v>207</v>
+      </c>
+      <c r="D82" t="s">
+        <v>280</v>
+      </c>
+      <c r="F82" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>134</v>
+      </c>
+      <c r="B83" t="s">
+        <v>109</v>
+      </c>
+      <c r="D83" t="s">
+        <v>158</v>
+      </c>
+      <c r="F83" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>135</v>
+      </c>
+      <c r="B84" t="s">
+        <v>110</v>
+      </c>
+      <c r="D84" t="s">
+        <v>159</v>
+      </c>
+      <c r="F84" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>136</v>
+      </c>
+      <c r="B85" t="s">
+        <v>111</v>
+      </c>
+      <c r="D85" t="s">
+        <v>160</v>
+      </c>
+      <c r="F85" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>366</v>
+      </c>
+      <c r="B86" t="s">
+        <v>369</v>
+      </c>
+      <c r="D86" t="s">
+        <v>372</v>
+      </c>
+      <c r="F86" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>367</v>
+      </c>
+      <c r="B87" t="s">
+        <v>370</v>
+      </c>
+      <c r="D87" t="s">
+        <v>373</v>
+      </c>
+      <c r="F87" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>368</v>
+      </c>
+      <c r="B88" t="s">
+        <v>371</v>
+      </c>
+      <c r="D88" t="s">
+        <v>374</v>
+      </c>
+      <c r="F88" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>137</v>
+      </c>
+      <c r="B89" t="s">
+        <v>112</v>
+      </c>
+      <c r="D89" t="s">
+        <v>161</v>
+      </c>
+      <c r="F89" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>138</v>
+      </c>
+      <c r="B90" t="s">
+        <v>113</v>
+      </c>
+      <c r="D90" t="s">
+        <v>162</v>
+      </c>
+      <c r="F90" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>139</v>
+      </c>
+      <c r="B91" t="s">
+        <v>114</v>
+      </c>
+      <c r="D91" t="s">
+        <v>163</v>
+      </c>
+      <c r="F91" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>140</v>
+      </c>
+      <c r="B92" t="s">
+        <v>115</v>
+      </c>
+      <c r="D92" t="s">
+        <v>164</v>
+      </c>
+      <c r="F92" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>141</v>
+      </c>
+      <c r="B93" t="s">
+        <v>116</v>
+      </c>
+      <c r="D93" t="s">
+        <v>165</v>
+      </c>
+      <c r="F93" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>142</v>
+      </c>
+      <c r="B94" t="s">
+        <v>117</v>
+      </c>
+      <c r="D94" t="s">
+        <v>166</v>
+      </c>
+      <c r="F94" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>402</v>
+      </c>
+      <c r="B95" t="s">
+        <v>208</v>
+      </c>
+      <c r="D95" t="s">
+        <v>281</v>
+      </c>
+      <c r="F95" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>403</v>
+      </c>
+      <c r="B96" t="s">
+        <v>209</v>
+      </c>
+      <c r="D96" t="s">
+        <v>282</v>
+      </c>
+      <c r="F96" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>404</v>
+      </c>
+      <c r="B97" t="s">
+        <v>210</v>
+      </c>
+      <c r="D97" t="s">
+        <v>283</v>
+      </c>
+      <c r="F97" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>143</v>
+      </c>
+      <c r="B98" t="s">
+        <v>118</v>
+      </c>
+      <c r="D98" t="s">
+        <v>167</v>
+      </c>
+      <c r="F98" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>144</v>
+      </c>
+      <c r="B99" t="s">
+        <v>119</v>
+      </c>
+      <c r="D99" t="s">
+        <v>168</v>
+      </c>
+      <c r="F99" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>145</v>
+      </c>
+      <c r="B100" t="s">
+        <v>120</v>
+      </c>
+      <c r="D100" t="s">
+        <v>169</v>
+      </c>
+      <c r="F100" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>146</v>
+      </c>
+      <c r="B101" t="s">
+        <v>121</v>
+      </c>
+      <c r="D101" t="s">
+        <v>170</v>
+      </c>
+      <c r="F101" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>147</v>
+      </c>
+      <c r="B102" t="s">
+        <v>122</v>
+      </c>
+      <c r="D102" t="s">
+        <v>171</v>
+      </c>
+      <c r="F102" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>148</v>
+      </c>
+      <c r="B103" t="s">
+        <v>123</v>
+      </c>
+      <c r="D103" t="s">
+        <v>172</v>
+      </c>
+      <c r="F103" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>405</v>
+      </c>
+      <c r="B104" t="s">
+        <v>211</v>
+      </c>
+      <c r="D104" t="s">
+        <v>284</v>
+      </c>
+      <c r="F104" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>406</v>
+      </c>
+      <c r="B105" t="s">
+        <v>212</v>
+      </c>
+      <c r="D105" t="s">
+        <v>285</v>
+      </c>
+      <c r="F105" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>407</v>
+      </c>
+      <c r="B106" t="s">
+        <v>213</v>
+      </c>
+      <c r="D106" t="s">
+        <v>286</v>
+      </c>
+      <c r="F106" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>408</v>
+      </c>
+      <c r="B107" t="s">
+        <v>214</v>
+      </c>
+      <c r="D107" t="s">
+        <v>287</v>
+      </c>
+      <c r="F107" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>409</v>
+      </c>
+      <c r="B108" t="s">
+        <v>215</v>
+      </c>
+      <c r="D108" t="s">
+        <v>288</v>
+      </c>
+      <c r="F108" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>410</v>
+      </c>
+      <c r="B109" t="s">
+        <v>216</v>
+      </c>
+      <c r="D109" t="s">
+        <v>289</v>
+      </c>
+      <c r="F109" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>411</v>
+      </c>
+      <c r="B110" t="s">
+        <v>217</v>
+      </c>
+      <c r="D110" t="s">
+        <v>290</v>
+      </c>
+      <c r="F110" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>412</v>
+      </c>
+      <c r="B111" t="s">
+        <v>218</v>
+      </c>
+      <c r="D111" t="s">
+        <v>291</v>
+      </c>
+      <c r="F111" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>413</v>
+      </c>
+      <c r="B112" t="s">
+        <v>219</v>
+      </c>
+      <c r="D112" t="s">
+        <v>292</v>
+      </c>
+      <c r="F112" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>414</v>
+      </c>
+      <c r="B113" t="s">
+        <v>220</v>
+      </c>
+      <c r="D113" t="s">
+        <v>293</v>
+      </c>
+      <c r="F113" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>415</v>
+      </c>
+      <c r="B114" t="s">
+        <v>221</v>
+      </c>
+      <c r="D114" t="s">
+        <v>294</v>
+      </c>
+      <c r="F114" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>416</v>
+      </c>
+      <c r="B115" t="s">
+        <v>222</v>
+      </c>
+      <c r="D115" t="s">
+        <v>295</v>
+      </c>
+      <c r="F115" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>417</v>
+      </c>
+      <c r="B116" t="s">
+        <v>223</v>
+      </c>
+      <c r="D116" t="s">
+        <v>296</v>
+      </c>
+      <c r="F116" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>418</v>
+      </c>
+      <c r="B117" t="s">
+        <v>224</v>
+      </c>
+      <c r="D117" t="s">
+        <v>297</v>
+      </c>
+      <c r="F117" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>419</v>
+      </c>
+      <c r="B118" t="s">
+        <v>225</v>
+      </c>
+      <c r="D118" t="s">
+        <v>298</v>
+      </c>
+      <c r="F118" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>420</v>
+      </c>
+      <c r="B119" t="s">
+        <v>226</v>
+      </c>
+      <c r="D119" t="s">
+        <v>299</v>
+      </c>
+      <c r="F119" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>421</v>
+      </c>
+      <c r="B120" t="s">
+        <v>227</v>
+      </c>
+      <c r="D120" t="s">
+        <v>300</v>
+      </c>
+      <c r="F120" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>422</v>
+      </c>
+      <c r="B121" t="s">
+        <v>228</v>
+      </c>
+      <c r="D121" t="s">
+        <v>301</v>
+      </c>
+      <c r="F121" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>423</v>
+      </c>
+      <c r="B122" t="s">
+        <v>229</v>
+      </c>
+      <c r="D122" t="s">
+        <v>302</v>
+      </c>
+      <c r="F122" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>424</v>
+      </c>
+      <c r="B123" t="s">
+        <v>230</v>
+      </c>
+      <c r="D123" t="s">
+        <v>303</v>
+      </c>
+      <c r="F123" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>425</v>
+      </c>
+      <c r="B124" t="s">
+        <v>231</v>
+      </c>
+      <c r="D124" t="s">
+        <v>304</v>
+      </c>
+      <c r="F124" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>426</v>
+      </c>
+      <c r="B125" t="s">
+        <v>232</v>
+      </c>
+      <c r="D125" t="s">
+        <v>305</v>
+      </c>
+      <c r="F125" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>427</v>
+      </c>
+      <c r="B126" t="s">
+        <v>233</v>
+      </c>
+      <c r="D126" t="s">
+        <v>306</v>
+      </c>
+      <c r="F126" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>428</v>
+      </c>
+      <c r="B127" t="s">
+        <v>234</v>
+      </c>
+      <c r="D127" t="s">
+        <v>307</v>
+      </c>
+      <c r="F127" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>429</v>
+      </c>
+      <c r="B128" t="s">
+        <v>235</v>
+      </c>
+      <c r="D128" t="s">
+        <v>308</v>
+      </c>
+      <c r="F128" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>430</v>
+      </c>
+      <c r="B129" t="s">
+        <v>236</v>
+      </c>
+      <c r="D129" t="s">
+        <v>309</v>
+      </c>
+      <c r="F129" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>431</v>
+      </c>
+      <c r="B130" t="s">
+        <v>237</v>
+      </c>
+      <c r="D130" t="s">
+        <v>310</v>
+      </c>
+      <c r="F130" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>432</v>
+      </c>
+      <c r="B131" t="s">
+        <v>238</v>
+      </c>
+      <c r="D131" t="s">
+        <v>311</v>
+      </c>
+      <c r="F131" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>433</v>
+      </c>
+      <c r="B132" t="s">
+        <v>239</v>
+      </c>
+      <c r="D132" t="s">
+        <v>312</v>
+      </c>
+      <c r="F132" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>434</v>
+      </c>
+      <c r="B133" t="s">
+        <v>240</v>
+      </c>
+      <c r="D133" t="s">
+        <v>313</v>
+      </c>
+      <c r="F133" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>435</v>
+      </c>
+      <c r="B134" t="s">
+        <v>241</v>
+      </c>
+      <c r="D134" t="s">
+        <v>314</v>
+      </c>
+      <c r="F134" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>436</v>
+      </c>
+      <c r="B135" t="s">
+        <v>242</v>
+      </c>
+      <c r="D135" t="s">
+        <v>315</v>
+      </c>
+      <c r="F135" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>437</v>
+      </c>
+      <c r="B136" t="s">
+        <v>243</v>
+      </c>
+      <c r="D136" t="s">
+        <v>316</v>
+      </c>
+      <c r="F136" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>149</v>
+      </c>
+      <c r="B137" t="s">
+        <v>124</v>
+      </c>
+      <c r="D137" t="s">
+        <v>173</v>
+      </c>
+      <c r="F137" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>150</v>
+      </c>
+      <c r="B138" t="s">
+        <v>125</v>
+      </c>
+      <c r="D138" t="s">
+        <v>174</v>
+      </c>
+      <c r="F138" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>151</v>
       </c>
-      <c r="B58" t="s">
-        <v>192</v>
-      </c>
-      <c r="D58" t="s">
-        <v>265</v>
-      </c>
-      <c r="F58" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>193</v>
-      </c>
-      <c r="D59" t="s">
-        <v>266</v>
-      </c>
-      <c r="F59" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>194</v>
-      </c>
-      <c r="D60" t="s">
-        <v>267</v>
-      </c>
-      <c r="F60" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>195</v>
-      </c>
-      <c r="D61" t="s">
-        <v>268</v>
-      </c>
-      <c r="F61" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>196</v>
-      </c>
-      <c r="D62" t="s">
-        <v>269</v>
-      </c>
-      <c r="F62" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>197</v>
-      </c>
-      <c r="D63" t="s">
-        <v>270</v>
-      </c>
-      <c r="F63" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>198</v>
-      </c>
-      <c r="D64" t="s">
-        <v>271</v>
-      </c>
-      <c r="F64" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>199</v>
-      </c>
-      <c r="D65" t="s">
-        <v>272</v>
-      </c>
-      <c r="F65" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>200</v>
-      </c>
-      <c r="D66" t="s">
-        <v>273</v>
-      </c>
-      <c r="F66" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>201</v>
-      </c>
-      <c r="D67" t="s">
-        <v>274</v>
-      </c>
-      <c r="F67" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>202</v>
-      </c>
-      <c r="D68" t="s">
-        <v>275</v>
-      </c>
-      <c r="F68" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>203</v>
-      </c>
-      <c r="D69" t="s">
-        <v>276</v>
-      </c>
-      <c r="F69" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>204</v>
-      </c>
-      <c r="D70" t="s">
-        <v>277</v>
-      </c>
-      <c r="F70" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
-        <v>205</v>
-      </c>
-      <c r="D71" t="s">
-        <v>278</v>
-      </c>
-      <c r="F71" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
-        <v>206</v>
-      </c>
-      <c r="D72" t="s">
-        <v>279</v>
-      </c>
-      <c r="F72" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>207</v>
-      </c>
-      <c r="D73" t="s">
-        <v>280</v>
-      </c>
-      <c r="F73" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>109</v>
-      </c>
-      <c r="D74" t="s">
-        <v>158</v>
-      </c>
-      <c r="F74" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
-        <v>110</v>
-      </c>
-      <c r="D75" t="s">
-        <v>159</v>
-      </c>
-      <c r="F75" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
-        <v>111</v>
-      </c>
-      <c r="D76" t="s">
-        <v>160</v>
-      </c>
-      <c r="F76" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
-        <v>112</v>
-      </c>
-      <c r="D77" t="s">
-        <v>161</v>
-      </c>
-      <c r="F77" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>113</v>
-      </c>
-      <c r="D78" t="s">
-        <v>162</v>
-      </c>
-      <c r="F78" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
-        <v>114</v>
-      </c>
-      <c r="D79" t="s">
-        <v>163</v>
-      </c>
-      <c r="F79" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>115</v>
-      </c>
-      <c r="D80" t="s">
-        <v>164</v>
-      </c>
-      <c r="F80" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
-        <v>116</v>
-      </c>
-      <c r="D81" t="s">
-        <v>165</v>
-      </c>
-      <c r="F81" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>117</v>
-      </c>
-      <c r="D82" t="s">
-        <v>166</v>
-      </c>
-      <c r="F82" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
-        <v>208</v>
-      </c>
-      <c r="D83" t="s">
-        <v>281</v>
-      </c>
-      <c r="F83" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>209</v>
-      </c>
-      <c r="D84" t="s">
-        <v>282</v>
-      </c>
-      <c r="F84" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>210</v>
-      </c>
-      <c r="D85" t="s">
-        <v>283</v>
-      </c>
-      <c r="F85" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
-        <v>118</v>
-      </c>
-      <c r="D86" t="s">
-        <v>167</v>
-      </c>
-      <c r="F86" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
-        <v>119</v>
-      </c>
-      <c r="D87" t="s">
-        <v>168</v>
-      </c>
-      <c r="F87" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
-        <v>120</v>
-      </c>
-      <c r="D88" t="s">
-        <v>169</v>
-      </c>
-      <c r="F88" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
-        <v>121</v>
-      </c>
-      <c r="D89" t="s">
-        <v>170</v>
-      </c>
-      <c r="F89" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
-        <v>122</v>
-      </c>
-      <c r="D90" t="s">
-        <v>171</v>
-      </c>
-      <c r="F90" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
-        <v>123</v>
-      </c>
-      <c r="D91" t="s">
-        <v>172</v>
-      </c>
-      <c r="F91" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
-        <v>211</v>
-      </c>
-      <c r="D92" t="s">
-        <v>284</v>
-      </c>
-      <c r="F92" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
-        <v>212</v>
-      </c>
-      <c r="D93" t="s">
-        <v>285</v>
-      </c>
-      <c r="F93" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
-        <v>213</v>
-      </c>
-      <c r="D94" t="s">
-        <v>286</v>
-      </c>
-      <c r="F94" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
-        <v>214</v>
-      </c>
-      <c r="D95" t="s">
-        <v>287</v>
-      </c>
-      <c r="F95" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
-        <v>215</v>
-      </c>
-      <c r="D96" t="s">
-        <v>288</v>
-      </c>
-      <c r="F96" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
-        <v>216</v>
-      </c>
-      <c r="D97" t="s">
-        <v>289</v>
-      </c>
-      <c r="F97" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B98" t="s">
-        <v>217</v>
-      </c>
-      <c r="D98" t="s">
-        <v>290</v>
-      </c>
-      <c r="F98" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
-        <v>218</v>
-      </c>
-      <c r="D99" t="s">
-        <v>291</v>
-      </c>
-      <c r="F99" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B100" t="s">
-        <v>219</v>
-      </c>
-      <c r="D100" t="s">
-        <v>292</v>
-      </c>
-      <c r="F100" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
-        <v>220</v>
-      </c>
-      <c r="D101" t="s">
-        <v>293</v>
-      </c>
-      <c r="F101" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B102" t="s">
-        <v>221</v>
-      </c>
-      <c r="D102" t="s">
-        <v>294</v>
-      </c>
-      <c r="F102" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B103" t="s">
-        <v>222</v>
-      </c>
-      <c r="D103" t="s">
-        <v>295</v>
-      </c>
-      <c r="F103" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B104" t="s">
-        <v>223</v>
-      </c>
-      <c r="D104" t="s">
-        <v>296</v>
-      </c>
-      <c r="F104" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
-        <v>224</v>
-      </c>
-      <c r="D105" t="s">
-        <v>297</v>
-      </c>
-      <c r="F105" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B106" t="s">
-        <v>225</v>
-      </c>
-      <c r="D106" t="s">
-        <v>298</v>
-      </c>
-      <c r="F106" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
-        <v>226</v>
-      </c>
-      <c r="D107" t="s">
-        <v>299</v>
-      </c>
-      <c r="F107" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B108" t="s">
-        <v>227</v>
-      </c>
-      <c r="D108" t="s">
-        <v>300</v>
-      </c>
-      <c r="F108" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
-        <v>228</v>
-      </c>
-      <c r="D109" t="s">
-        <v>301</v>
-      </c>
-      <c r="F109" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
-        <v>229</v>
-      </c>
-      <c r="D110" t="s">
-        <v>302</v>
-      </c>
-      <c r="F110" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B111" t="s">
-        <v>230</v>
-      </c>
-      <c r="D111" t="s">
-        <v>303</v>
-      </c>
-      <c r="F111" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B112" t="s">
-        <v>231</v>
-      </c>
-      <c r="D112" t="s">
-        <v>304</v>
-      </c>
-      <c r="F112" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B113" t="s">
-        <v>232</v>
-      </c>
-      <c r="D113" t="s">
-        <v>305</v>
-      </c>
-      <c r="F113" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B114" t="s">
-        <v>233</v>
-      </c>
-      <c r="D114" t="s">
-        <v>306</v>
-      </c>
-      <c r="F114" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B115" t="s">
-        <v>234</v>
-      </c>
-      <c r="D115" t="s">
-        <v>307</v>
-      </c>
-      <c r="F115" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B116" t="s">
-        <v>235</v>
-      </c>
-      <c r="D116" t="s">
-        <v>308</v>
-      </c>
-      <c r="F116" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B117" t="s">
-        <v>236</v>
-      </c>
-      <c r="D117" t="s">
-        <v>309</v>
-      </c>
-      <c r="F117" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B118" t="s">
-        <v>237</v>
-      </c>
-      <c r="D118" t="s">
-        <v>310</v>
-      </c>
-      <c r="F118" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B119" t="s">
-        <v>238</v>
-      </c>
-      <c r="D119" t="s">
-        <v>311</v>
-      </c>
-      <c r="F119" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B120" t="s">
-        <v>239</v>
-      </c>
-      <c r="D120" t="s">
-        <v>312</v>
-      </c>
-      <c r="F120" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B121" t="s">
-        <v>240</v>
-      </c>
-      <c r="D121" t="s">
-        <v>313</v>
-      </c>
-      <c r="F121" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B122" t="s">
-        <v>241</v>
-      </c>
-      <c r="D122" t="s">
-        <v>314</v>
-      </c>
-      <c r="F122" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B123" t="s">
-        <v>242</v>
-      </c>
-      <c r="D123" t="s">
-        <v>315</v>
-      </c>
-      <c r="F123" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B124" t="s">
-        <v>243</v>
-      </c>
-      <c r="D124" t="s">
-        <v>316</v>
-      </c>
-      <c r="F124" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B125" t="s">
-        <v>124</v>
-      </c>
-      <c r="D125" t="s">
-        <v>173</v>
-      </c>
-      <c r="F125" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B126" t="s">
-        <v>125</v>
-      </c>
-      <c r="D126" t="s">
-        <v>174</v>
-      </c>
-      <c r="F126" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B127" t="s">
+      <c r="B139" t="s">
         <v>126</v>
       </c>
-      <c r="D127" t="s">
+      <c r="D139" t="s">
         <v>175</v>
       </c>
-      <c r="F127" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B128" t="s">
+      <c r="F139" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>438</v>
+      </c>
+      <c r="B140" t="s">
         <v>244</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D140" t="s">
         <v>317</v>
       </c>
-      <c r="F128" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B129" t="s">
+      <c r="F140" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>439</v>
+      </c>
+      <c r="B141" t="s">
         <v>245</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D141" t="s">
         <v>318</v>
       </c>
-      <c r="F129" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B130" t="s">
+      <c r="F141" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>440</v>
+      </c>
+      <c r="B142" t="s">
         <v>246</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D142" t="s">
         <v>319</v>
       </c>
-      <c r="F130" s="4">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B131" t="s">
+      <c r="F142" s="4">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
         <v>320</v>
       </c>
-      <c r="D131" t="s">
+      <c r="D143" t="s">
         <v>321</v>
       </c>
-      <c r="E131" s="2" t="s">
+      <c r="E143" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="F131" s="4">
+      <c r="F143" s="4">
         <v>43333</v>
       </c>
     </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B132" t="s">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>441</v>
+      </c>
+      <c r="B144" t="s">
         <v>323</v>
       </c>
-      <c r="D132" s="2" t="s">
+      <c r="D144" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="E132" t="s">
+      <c r="E144" t="s">
         <v>325</v>
       </c>
-      <c r="F132" s="4">
+      <c r="F144" s="4">
         <v>43335</v>
       </c>
     </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B133" t="s">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>442</v>
+      </c>
+      <c r="B145" t="s">
         <v>326</v>
       </c>
-      <c r="D133" t="s">
+      <c r="D145" t="s">
         <v>327</v>
       </c>
-      <c r="F133" s="4">
+      <c r="F145" s="4">
         <v>43382</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
+        <v>337</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="F146" s="4">
+        <v>43539</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
+        <v>334</v>
+      </c>
+      <c r="D147" t="s">
+        <v>336</v>
+      </c>
+      <c r="F147" s="4">
+        <v>43559</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>443</v>
+      </c>
+      <c r="B148" t="s">
+        <v>335</v>
+      </c>
+      <c r="D148" t="s">
+        <v>336</v>
+      </c>
+      <c r="F148" s="4">
+        <v>43559</v>
       </c>
     </row>
   </sheetData>
@@ -3142,12 +3899,13 @@
     <hyperlink ref="E25" r:id="rId13" display="https://doi.org/10.1093/nar/gkw1039"/>
     <hyperlink ref="E33" r:id="rId14"/>
     <hyperlink ref="E34" r:id="rId15"/>
-    <hyperlink ref="E131" r:id="rId16"/>
-    <hyperlink ref="D132" r:id="rId17"/>
+    <hyperlink ref="E143" r:id="rId16"/>
+    <hyperlink ref="D144" r:id="rId17"/>
     <hyperlink ref="D34" r:id="rId18"/>
+    <hyperlink ref="D146" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 

</xml_diff>